<commit_message>
Only one speed condition, 4 loops
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A099E01A-AC9D-A64B-98EA-37F71A2F509E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2FDB92-5579-2D4A-BA0C-1C9DBA327FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="1400" windowWidth="27640" windowHeight="15880" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
+    <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15880" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,7 +465,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,10 +495,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C2">
         <v>99</v>
@@ -518,19 +518,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C3">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>3</v>
@@ -541,22 +541,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="G4">
         <v>6</v>
@@ -564,19 +564,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -587,10 +587,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="C6">
         <v>99</v>
@@ -599,173 +599,35 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C7">
         <v>99</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
-        <v>99</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>99</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10">
-        <v>99</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>3</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>99</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12">
-        <v>2</v>
-      </c>
-      <c r="C12">
-        <v>99</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>3</v>
-      </c>
-      <c r="G12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>99</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>4</v>
-      </c>
-      <c r="F13">
-        <v>3</v>
-      </c>
-      <c r="G13">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed speed to 1 for rotation and 2 for mask
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E2FDB92-5579-2D4A-BA0C-1C9DBA327FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3459AF65-486C-A144-BEC4-5AA2C41535F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15880" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,10 +495,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>99</v>
@@ -518,10 +518,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -541,10 +541,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>99</v>
@@ -564,10 +564,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>99</v>
@@ -587,10 +587,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="B6">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>99</v>
@@ -610,10 +610,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>99</v>

</xml_diff>

<commit_message>
changed speed to 2 for both
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3459AF65-486C-A144-BEC4-5AA2C41535F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB4979D-6328-DD47-8861-77DA3EFF4EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15880" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -465,7 +465,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,7 +495,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -518,7 +518,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -610,7 +610,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>2</v>

</xml_diff>

<commit_message>
Made Rotation slightly slower
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB4979D-6328-DD47-8861-77DA3EFF4EF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D6D0E6-58CC-6B40-8EEC-911A0E9D5C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15880" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -36,13 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>nr</t>
-  </si>
-  <si>
-    <t>nm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>v</t>
   </si>
@@ -465,169 +459,127 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>99</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>99</v>
       </c>
-      <c r="D2">
+      <c r="B4">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2.5</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>99</v>
+      </c>
+      <c r="B5">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
+      <c r="C5">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>99</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>4</v>
-      </c>
-      <c r="F4">
-        <v>2.5</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>99</v>
-      </c>
       <c r="D5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>6</v>
       </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>99</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>99</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
       <c r="C7">
-        <v>99</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
         <v>15</v>
       </c>
     </row>
@@ -651,7 +603,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid variable name" error="Variable names need to start with a letter or an underscore (_), followed by only letters, numbers and underscores." sqref="A1:E1" xr:uid="{81FE39FE-1437-A54A-87EA-65F094256462}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid variable name" error="Variable names need to start with a letter or an underscore (_), followed by only letters, numbers and underscores." sqref="A1:C1" xr:uid="{81FE39FE-1437-A54A-87EA-65F094256462}">
       <formula1>AND(ISNUMBER(SUMPRODUCT(SEARCH(MID(A1,ROW(INDIRECT("1:"&amp;LEN(A1))),1),"0123456789abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ_"))),ISNUMBER(SEARCH(LEFT(A1,1),"abcdefghijklmnopqrstuvwxyzABCDEFGHIJKLMNOPQRSTUVWXYZ_")),NOT(ISNUMBER(SEARCH("~*",A1))))</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
made all trials nonlinear and proximity = 2 to test
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238A6A87-A405-F743-A71C-937836DE3AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896B72D0-2F83-DA46-B8BE-5A9661117AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15880" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,13 +486,13 @@
         <v>99</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -503,13 +503,13 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>6</v>
@@ -520,13 +520,13 @@
         <v>99</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>6</v>
@@ -537,13 +537,13 @@
         <v>99</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -554,13 +554,13 @@
         <v>99</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -577,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
         <v>6</v>

</xml_diff>

<commit_message>
changed the first instructions to be inside the circle
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F681E140-DDE1-C94D-A5D9-5542C4BFC26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7465ED64-0EA4-1342-8C7F-E0F8933716A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15880" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,7 +498,7 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -518,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>6</v>
@@ -538,7 +538,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4">
         <v>6</v>
@@ -558,7 +558,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>15</v>

</xml_diff>

<commit_message>
changed order of s
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1951311D-04D9-654D-AE6A-85C9F78CE02A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{838845B9-ECDE-5847-ABAB-7F824F0D466C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1000" windowWidth="27640" windowHeight="15880" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
+    <workbookView xWindow="5960" yWindow="1460" windowWidth="10000" windowHeight="15880" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -462,7 +462,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,7 +495,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -515,7 +515,7 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -535,7 +535,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -555,7 +555,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -575,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D6">
         <v>3</v>

</xml_diff>

<commit_message>
chagend 15 dots to position 0
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CBE3F6-D1C9-EA44-A9F0-90A4A9319D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D723DD-AE1C-6B43-8D3B-B0F09297767D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>3</v>

</xml_diff>

<commit_message>
changed c to cc
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D723DD-AE1C-6B43-8D3B-B0F09297767D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B37924C-10CA-9F4D-A82E-3E4323F01644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
+    <workbookView xWindow="5960" yWindow="1460" windowWidth="10000" windowHeight="15880" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <t>q</t>
   </si>
   <si>
-    <t>c</t>
+    <t>cc</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,7 +524,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>3</v>

</xml_diff>

<commit_message>
changed cc back to c
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48787F4-5AF2-6B4A-A0FA-FA97A6F76BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E79D0E-AF8C-724A-834D-92CEBE592871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <t>q</t>
   </si>
   <si>
-    <t>cc</t>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
make rotation switch circleCount instead of Mask
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FDD75A-66AA-E142-8619-701EC37C6C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4DDC13-119D-E642-B7F8-E8DF646B00B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,7 +530,7 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -547,7 +547,7 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Split up c into cR and cM
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4DDC13-119D-E642-B7F8-E8DF646B00B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DFFEC9-7D06-6D4E-B1F8-434EB97B8F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>v</t>
   </si>
@@ -50,7 +50,10 @@
     <t>q</t>
   </si>
   <si>
-    <t>c</t>
+    <t>cR</t>
+  </si>
+  <si>
+    <t>cM</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,7 +483,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -498,6 +503,9 @@
       <c r="E2">
         <v>6</v>
       </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -513,6 +521,9 @@
         <v>3</v>
       </c>
       <c r="E3">
+        <v>6</v>
+      </c>
+      <c r="F3">
         <v>6</v>
       </c>
     </row>
@@ -532,6 +543,9 @@
       <c r="E4">
         <v>15</v>
       </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -549,6 +563,9 @@
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -566,6 +583,9 @@
       <c r="E6">
         <v>6</v>
       </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -581,6 +601,9 @@
         <v>3</v>
       </c>
       <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
replaced circleCount with cM in Mask begin Routine loops
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DFFEC9-7D06-6D4E-B1F8-434EB97B8F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38409168-B9B1-DC43-92BC-2CD530526228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E7" sqref="E7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Put one dot all the way in the back, added second proximity condition
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38409168-B9B1-DC43-92BC-2CD530526228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEC848A-2AC8-3D45-BCF1-EB81A5D34012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>v</t>
   </si>
@@ -50,10 +50,7 @@
     <t>q</t>
   </si>
   <si>
-    <t>cR</t>
-  </si>
-  <si>
-    <t>cM</t>
+    <t>c</t>
   </si>
 </sst>
 </file>
@@ -462,7 +459,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:F7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -483,9 +480,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -503,9 +498,6 @@
       <c r="E2">
         <v>6</v>
       </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
@@ -523,9 +515,6 @@
       <c r="E3">
         <v>6</v>
       </c>
-      <c r="F3">
-        <v>6</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -543,9 +532,6 @@
       <c r="E4">
         <v>15</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -555,16 +541,13 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -583,9 +566,6 @@
       <c r="E6">
         <v>6</v>
       </c>
-      <c r="F6">
-        <v>6</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -601,9 +581,6 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="F7">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changed q to 1,3,6 instead of 2,3,4
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEC848A-2AC8-3D45-BCF1-EB81A5D34012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99CE60F-5DC6-7947-AA49-DBCAB945E260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>6</v>
@@ -561,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
         <v>6</v>

</xml_diff>

<commit_message>
changed q back to 2,3,4
</commit_message>
<xml_diff>
--- a/Book5.xlsx
+++ b/Book5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janthiel/Downloads/CircleBounceNew/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99CE60F-5DC6-7947-AA49-DBCAB945E260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99B5593-B5A4-F848-918C-2AAC240FF363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{0E0FE66A-1B4A-C443-A9A7-91F18123157B}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,7 +544,7 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <v>6</v>
@@ -561,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>6</v>

</xml_diff>